<commit_message>
Update files on the sprint1
</commit_message>
<xml_diff>
--- a/SE2223_60157_60201_60226_60479_60749/Phase_2/Sprint1/Burndown Chart.xlsx
+++ b/SE2223_60157_60201_60226_60479_60749/Phase_2/Sprint1/Burndown Chart.xlsx
@@ -350,11 +350,11 @@
           </c:val>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="1484383969"/>
-        <c:axId val="345454559"/>
+        <c:axId val="391436782"/>
+        <c:axId val="1486345295"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="1484383969"/>
+        <c:axId val="391436782"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -406,10 +406,10 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="345454559"/>
+        <c:crossAx val="1486345295"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="345454559"/>
+        <c:axId val="1486345295"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -484,7 +484,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1484383969"/>
+        <c:crossAx val="391436782"/>
       </c:valAx>
     </c:plotArea>
     <c:legend>

</xml_diff>